<commit_message>
Changed (corrected) data validation rule for 2 fields
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet1.xlsx
+++ b/xlsx/sample-spreadsheet1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709838A9-12B3-4B96-A60A-476D699484E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D32B22-EED5-44F3-ACA8-6205619D45A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="827">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="833">
   <si>
     <t>Municipality</t>
   </si>
@@ -582,9 +582,6 @@
     <t>Location Type</t>
   </si>
   <si>
-    <t>Facility</t>
-  </si>
-  <si>
     <t>Roadway</t>
   </si>
   <si>
@@ -2512,6 +2509,27 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>Sunny (1)</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Party Cloudy (2)</t>
+  </si>
+  <si>
+    <t>Overcast (3)</t>
+  </si>
+  <si>
+    <t>Precipitation (4)</t>
+  </si>
+  <si>
+    <t>No Data (99)</t>
+  </si>
+  <si>
+    <t>Bicycle/Pedestrian Facility</t>
   </si>
 </sst>
 </file>
@@ -2583,6 +2601,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2592,7 +2611,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2623,12 +2641,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}" name="Table5" displayName="Table5" ref="D1:F273" totalsRowShown="0">
-  <autoFilter ref="D1:F273" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}" name="Table5" displayName="Table5" ref="D1:G273" totalsRowShown="0">
+  <autoFilter ref="D1:G273" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{09935779-A7F4-4E95-BF0B-6D7F0A5AF862}" name="Count Location Description"/>
     <tableColumn id="2" xr3:uid="{588C097D-696D-4C7A-AB98-CC5016F219D2}" name="Street #1 Name"/>
     <tableColumn id="3" xr3:uid="{CA556A4C-1BD7-4427-8132-618C09C12162}" name="Street #2 Name"/>
+    <tableColumn id="4" xr3:uid="{C9E4663B-CFA0-49B0-ABFE-EA028F045F02}" name="Column1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2933,14 +2952,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D396DD5C-31B0-418A-83C6-51CCF2B5706A}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
     <col min="3" max="3" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.140625" customWidth="1"/>
@@ -2951,14 +2970,14 @@
         <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="B2" s="10">
+        <v>812</v>
+      </c>
+      <c r="B2" s="7">
         <v>45212</v>
       </c>
       <c r="C2" s="3">
@@ -2978,18 +2997,18 @@
         <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
+        <v>184</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -3001,82 +3020,76 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B7" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="B8" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="B9" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="B11" t="s">
-        <v>706</v>
+        <v>813</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="B12" t="s">
-        <v>708</v>
+        <v>814</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>812</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="A14" s="8" t="s">
+        <v>811</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3084,10 +3097,16 @@
     <mergeCell ref="A15:D16"/>
     <mergeCell ref="B5:D5"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{DE9B4560-966C-4313-BEB6-AAD929529159}">
+      <formula1>-100</formula1>
+      <formula2>120</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBF8E227-3C60-4987-AFCD-93955E6231E2}">
           <x14:formula1>
             <xm:f>Columns!$A$2:$A$57</xm:f>
@@ -3122,7 +3141,13 @@
           <x14:formula1>
             <xm:f>Columns!$F$2:$F$160</xm:f>
           </x14:formula1>
-          <xm:sqref>B9:B12</xm:sqref>
+          <xm:sqref>B9:B10</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{673A9766-EB25-4266-BAB5-BD22FA753598}">
+          <x14:formula1>
+            <xm:f>Columns!$G$2:$G$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B12</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3134,7 +3159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF117DD8-8B54-44CC-AA12-FC16BF191D23}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -3145,25 +3170,25 @@
   <sheetData>
     <row r="1" spans="1:8" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>824</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>825</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>58</v>
@@ -3264,25 +3289,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>824</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>825</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>58</v>
@@ -3371,25 +3396,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>824</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>825</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>58</v>
@@ -3477,25 +3502,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>824</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>825</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>58</v>
@@ -3583,25 +3608,25 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>819</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>821</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>820</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>822</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>824</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>825</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>58</v>
@@ -3674,23 +3699,24 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92867D1-D2E9-42B4-B903-CE81613CFB5C}">
-  <dimension ref="A1:F273"/>
+  <dimension ref="A1:G273"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F160"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="101" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3701,56 +3727,65 @@
         <v>57</v>
       </c>
       <c r="D1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E1" t="s">
+        <v>456</v>
+      </c>
+      <c r="F1" t="s">
         <v>457</v>
       </c>
-      <c r="F1" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>183</v>
+        <v>832</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
       </c>
       <c r="D2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="F2" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>705</v>
+      </c>
+      <c r="G2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C3" t="s">
         <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F3" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>706</v>
+      </c>
+      <c r="G3" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3758,16 +3793,19 @@
         <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E4" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F4" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>707</v>
+      </c>
+      <c r="G4" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3775,16 +3813,19 @@
         <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="F5" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>464</v>
+      </c>
+      <c r="G5" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3792,16 +3833,19 @@
         <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F6" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+      <c r="G6" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3809,16 +3853,16 @@
         <v>65</v>
       </c>
       <c r="D7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F7" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3826,16 +3870,16 @@
         <v>66</v>
       </c>
       <c r="D8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E8" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="F8" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3843,16 +3887,16 @@
         <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="F9" t="s">
-        <v>710</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3863,13 +3907,13 @@
         <v>64</v>
       </c>
       <c r="E10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F10" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3877,16 +3921,16 @@
         <v>69</v>
       </c>
       <c r="D11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E11" t="s">
         <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3894,16 +3938,16 @@
         <v>70</v>
       </c>
       <c r="D12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E12" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F12" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3911,16 +3955,16 @@
         <v>71</v>
       </c>
       <c r="D13" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E13" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="F13" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3928,16 +3972,16 @@
         <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F14" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3945,16 +3989,16 @@
         <v>73</v>
       </c>
       <c r="D15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E15" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F15" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -3962,13 +4006,13 @@
         <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E16" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F16" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -3979,13 +4023,13 @@
         <v>75</v>
       </c>
       <c r="D17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E17" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F17" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -3996,13 +4040,13 @@
         <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F18" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4013,13 +4057,13 @@
         <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E19" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F19" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4030,13 +4074,13 @@
         <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E20" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F20" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4047,13 +4091,13 @@
         <v>79</v>
       </c>
       <c r="D21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E21" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F21" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4064,13 +4108,13 @@
         <v>80</v>
       </c>
       <c r="D22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E22" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F22" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4081,13 +4125,13 @@
         <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E23" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F23" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4098,13 +4142,13 @@
         <v>82</v>
       </c>
       <c r="D24" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E24" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F24" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4115,13 +4159,13 @@
         <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E25" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F25" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4132,13 +4176,13 @@
         <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E26" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F26" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4149,13 +4193,13 @@
         <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E27" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F27" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4166,13 +4210,13 @@
         <v>86</v>
       </c>
       <c r="D28" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E28" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F28" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4183,13 +4227,13 @@
         <v>87</v>
       </c>
       <c r="D29" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E29" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F29" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4200,13 +4244,13 @@
         <v>88</v>
       </c>
       <c r="D30" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E30" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F30" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4217,13 +4261,13 @@
         <v>89</v>
       </c>
       <c r="D31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E31" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F31" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4234,13 +4278,13 @@
         <v>90</v>
       </c>
       <c r="D32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E32" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F32" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4251,13 +4295,13 @@
         <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E33" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F33" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4268,13 +4312,13 @@
         <v>92</v>
       </c>
       <c r="D34" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E34" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F34" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -4285,13 +4329,13 @@
         <v>93</v>
       </c>
       <c r="D35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E35" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F35" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4302,13 +4346,13 @@
         <v>94</v>
       </c>
       <c r="D36" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E36" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F36" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -4319,13 +4363,13 @@
         <v>95</v>
       </c>
       <c r="D37" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E37" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F37" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -4336,13 +4380,13 @@
         <v>96</v>
       </c>
       <c r="D38" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E38" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F38" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4353,13 +4397,13 @@
         <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E39" t="s">
         <v>77</v>
       </c>
       <c r="F39" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -4370,13 +4414,13 @@
         <v>98</v>
       </c>
       <c r="D40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E40" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F40" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -4387,13 +4431,13 @@
         <v>99</v>
       </c>
       <c r="D41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E41" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F41" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -4404,13 +4448,13 @@
         <v>100</v>
       </c>
       <c r="D42" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E42" t="s">
         <v>82</v>
       </c>
       <c r="F42" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -4421,13 +4465,13 @@
         <v>101</v>
       </c>
       <c r="D43" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E43" t="s">
         <v>84</v>
       </c>
       <c r="F43" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -4438,13 +4482,13 @@
         <v>102</v>
       </c>
       <c r="D44" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E44" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F44" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -4455,13 +4499,13 @@
         <v>103</v>
       </c>
       <c r="D45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E45" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F45" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -4472,13 +4516,13 @@
         <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E46" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F46" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -4489,13 +4533,13 @@
         <v>105</v>
       </c>
       <c r="D47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E47" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F47" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -4506,10 +4550,10 @@
         <v>106</v>
       </c>
       <c r="D48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E48" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F48" t="s">
         <v>105</v>
@@ -4523,13 +4567,13 @@
         <v>107</v>
       </c>
       <c r="D49" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E49" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F49" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -4540,13 +4584,13 @@
         <v>108</v>
       </c>
       <c r="D50" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E50" t="s">
         <v>90</v>
       </c>
       <c r="F50" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -4557,13 +4601,13 @@
         <v>109</v>
       </c>
       <c r="D51" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E51" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F51" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -4574,13 +4618,13 @@
         <v>110</v>
       </c>
       <c r="D52" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E52" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F52" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -4591,13 +4635,13 @@
         <v>111</v>
       </c>
       <c r="D53" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E53" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F53" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -4608,13 +4652,13 @@
         <v>112</v>
       </c>
       <c r="D54" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E54" t="s">
         <v>95</v>
       </c>
       <c r="F54" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -4625,13 +4669,13 @@
         <v>113</v>
       </c>
       <c r="D55" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E55" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F55" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -4642,13 +4686,13 @@
         <v>114</v>
       </c>
       <c r="D56" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E56" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F56" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -4659,13 +4703,13 @@
         <v>115</v>
       </c>
       <c r="D57" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E57" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F57" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -4673,13 +4717,13 @@
         <v>116</v>
       </c>
       <c r="D58" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E58" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F58" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -4687,13 +4731,13 @@
         <v>117</v>
       </c>
       <c r="D59" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E59" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F59" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -4701,13 +4745,13 @@
         <v>118</v>
       </c>
       <c r="D60" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E60" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F60" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -4715,13 +4759,13 @@
         <v>119</v>
       </c>
       <c r="D61" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E61" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F61" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -4729,13 +4773,13 @@
         <v>120</v>
       </c>
       <c r="D62" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E62" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F62" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -4743,13 +4787,13 @@
         <v>121</v>
       </c>
       <c r="D63" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E63" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F63" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -4757,13 +4801,13 @@
         <v>122</v>
       </c>
       <c r="D64" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E64" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F64" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
@@ -4771,13 +4815,13 @@
         <v>123</v>
       </c>
       <c r="D65" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E65" t="s">
         <v>105</v>
       </c>
       <c r="F65" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
@@ -4785,13 +4829,13 @@
         <v>124</v>
       </c>
       <c r="D66" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E66" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F66" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
@@ -4799,13 +4843,13 @@
         <v>125</v>
       </c>
       <c r="D67" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E67" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F67" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.25">
@@ -4813,13 +4857,13 @@
         <v>126</v>
       </c>
       <c r="D68" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E68" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F68" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.25">
@@ -4827,13 +4871,13 @@
         <v>127</v>
       </c>
       <c r="D69" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E69" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F69" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.25">
@@ -4841,13 +4885,13 @@
         <v>128</v>
       </c>
       <c r="D70" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E70" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F70" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.25">
@@ -4855,13 +4899,13 @@
         <v>129</v>
       </c>
       <c r="D71" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E71" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F71" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.25">
@@ -4869,13 +4913,13 @@
         <v>130</v>
       </c>
       <c r="D72" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E72" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F72" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.25">
@@ -4883,13 +4927,13 @@
         <v>131</v>
       </c>
       <c r="D73" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E73" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F73" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.25">
@@ -4897,13 +4941,13 @@
         <v>132</v>
       </c>
       <c r="D74" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E74" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F74" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.25">
@@ -4911,13 +4955,13 @@
         <v>133</v>
       </c>
       <c r="D75" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E75" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F75" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
@@ -4925,13 +4969,13 @@
         <v>134</v>
       </c>
       <c r="D76" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E76" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F76" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
@@ -4939,13 +4983,13 @@
         <v>135</v>
       </c>
       <c r="D77" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E77" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F77" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
@@ -4953,13 +4997,13 @@
         <v>136</v>
       </c>
       <c r="D78" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E78" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F78" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
@@ -4967,13 +5011,13 @@
         <v>137</v>
       </c>
       <c r="D79" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E79" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F79" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
@@ -4981,13 +5025,13 @@
         <v>138</v>
       </c>
       <c r="D80" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E80" t="s">
         <v>107</v>
       </c>
       <c r="F80" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
@@ -4995,13 +5039,13 @@
         <v>139</v>
       </c>
       <c r="D81" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E81" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F81" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.25">
@@ -5009,13 +5053,13 @@
         <v>140</v>
       </c>
       <c r="D82" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E82" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F82" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="83" spans="3:6" x14ac:dyDescent="0.25">
@@ -5023,13 +5067,13 @@
         <v>141</v>
       </c>
       <c r="D83" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E83" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F83" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="84" spans="3:6" x14ac:dyDescent="0.25">
@@ -5037,13 +5081,13 @@
         <v>142</v>
       </c>
       <c r="D84" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E84" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F84" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="85" spans="3:6" x14ac:dyDescent="0.25">
@@ -5051,13 +5095,13 @@
         <v>143</v>
       </c>
       <c r="D85" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E85" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F85" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
     </row>
     <row r="86" spans="3:6" x14ac:dyDescent="0.25">
@@ -5065,13 +5109,13 @@
         <v>144</v>
       </c>
       <c r="D86" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E86" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F86" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
     </row>
     <row r="87" spans="3:6" x14ac:dyDescent="0.25">
@@ -5079,13 +5123,13 @@
         <v>145</v>
       </c>
       <c r="D87" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E87" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F87" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="88" spans="3:6" x14ac:dyDescent="0.25">
@@ -5093,13 +5137,13 @@
         <v>146</v>
       </c>
       <c r="D88" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E88" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F88" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="89" spans="3:6" x14ac:dyDescent="0.25">
@@ -5107,13 +5151,13 @@
         <v>147</v>
       </c>
       <c r="D89" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E89" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F89" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="90" spans="3:6" x14ac:dyDescent="0.25">
@@ -5121,13 +5165,13 @@
         <v>148</v>
       </c>
       <c r="D90" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E90" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F90" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="91" spans="3:6" x14ac:dyDescent="0.25">
@@ -5135,13 +5179,13 @@
         <v>149</v>
       </c>
       <c r="D91" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E91" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F91" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
     </row>
     <row r="92" spans="3:6" x14ac:dyDescent="0.25">
@@ -5149,13 +5193,13 @@
         <v>150</v>
       </c>
       <c r="D92" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E92" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F92" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="93" spans="3:6" x14ac:dyDescent="0.25">
@@ -5163,13 +5207,13 @@
         <v>151</v>
       </c>
       <c r="D93" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E93" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F93" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
     </row>
     <row r="94" spans="3:6" x14ac:dyDescent="0.25">
@@ -5177,13 +5221,13 @@
         <v>152</v>
       </c>
       <c r="D94" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E94" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F94" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="95" spans="3:6" x14ac:dyDescent="0.25">
@@ -5191,13 +5235,13 @@
         <v>153</v>
       </c>
       <c r="D95" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E95" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F95" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
     </row>
     <row r="96" spans="3:6" x14ac:dyDescent="0.25">
@@ -5205,13 +5249,13 @@
         <v>154</v>
       </c>
       <c r="D96" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E96" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F96" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="97" spans="3:6" x14ac:dyDescent="0.25">
@@ -5219,13 +5263,13 @@
         <v>155</v>
       </c>
       <c r="D97" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E97" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F97" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
     </row>
     <row r="98" spans="3:6" x14ac:dyDescent="0.25">
@@ -5233,13 +5277,13 @@
         <v>156</v>
       </c>
       <c r="D98" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E98" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F98" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
     </row>
     <row r="99" spans="3:6" x14ac:dyDescent="0.25">
@@ -5247,13 +5291,13 @@
         <v>157</v>
       </c>
       <c r="D99" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E99" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F99" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="100" spans="3:6" x14ac:dyDescent="0.25">
@@ -5261,13 +5305,13 @@
         <v>158</v>
       </c>
       <c r="D100" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E100" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F100" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
     </row>
     <row r="101" spans="3:6" x14ac:dyDescent="0.25">
@@ -5275,13 +5319,13 @@
         <v>159</v>
       </c>
       <c r="D101" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E101" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F101" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
     </row>
     <row r="102" spans="3:6" x14ac:dyDescent="0.25">
@@ -5289,13 +5333,13 @@
         <v>160</v>
       </c>
       <c r="D102" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E102" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F102" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="103" spans="3:6" x14ac:dyDescent="0.25">
@@ -5303,13 +5347,13 @@
         <v>161</v>
       </c>
       <c r="D103" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E103" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F103" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
     </row>
     <row r="104" spans="3:6" x14ac:dyDescent="0.25">
@@ -5317,13 +5361,13 @@
         <v>162</v>
       </c>
       <c r="D104" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E104" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F104" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
     </row>
     <row r="105" spans="3:6" x14ac:dyDescent="0.25">
@@ -5331,13 +5375,13 @@
         <v>163</v>
       </c>
       <c r="D105" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E105" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F105" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
     </row>
     <row r="106" spans="3:6" x14ac:dyDescent="0.25">
@@ -5345,13 +5389,13 @@
         <v>164</v>
       </c>
       <c r="D106" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E106" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F106" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
     </row>
     <row r="107" spans="3:6" x14ac:dyDescent="0.25">
@@ -5359,13 +5403,13 @@
         <v>165</v>
       </c>
       <c r="D107" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E107" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F107" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
     </row>
     <row r="108" spans="3:6" x14ac:dyDescent="0.25">
@@ -5373,13 +5417,13 @@
         <v>166</v>
       </c>
       <c r="D108" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E108" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F108" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
     </row>
     <row r="109" spans="3:6" x14ac:dyDescent="0.25">
@@ -5387,13 +5431,13 @@
         <v>167</v>
       </c>
       <c r="D109" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E109" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F109" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
     </row>
     <row r="110" spans="3:6" x14ac:dyDescent="0.25">
@@ -5401,13 +5445,13 @@
         <v>168</v>
       </c>
       <c r="D110" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E110" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F110" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
     </row>
     <row r="111" spans="3:6" x14ac:dyDescent="0.25">
@@ -5415,13 +5459,13 @@
         <v>169</v>
       </c>
       <c r="D111" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E111" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F111" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
     </row>
     <row r="112" spans="3:6" x14ac:dyDescent="0.25">
@@ -5429,13 +5473,13 @@
         <v>170</v>
       </c>
       <c r="D112" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E112" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F112" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
     </row>
     <row r="113" spans="3:6" x14ac:dyDescent="0.25">
@@ -5443,13 +5487,13 @@
         <v>171</v>
       </c>
       <c r="D113" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E113" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F113" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
     </row>
     <row r="114" spans="3:6" x14ac:dyDescent="0.25">
@@ -5457,13 +5501,13 @@
         <v>172</v>
       </c>
       <c r="D114" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E114" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F114" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
     </row>
     <row r="115" spans="3:6" x14ac:dyDescent="0.25">
@@ -5471,13 +5515,13 @@
         <v>173</v>
       </c>
       <c r="D115" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E115" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F115" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
     </row>
     <row r="116" spans="3:6" x14ac:dyDescent="0.25">
@@ -5485,13 +5529,13 @@
         <v>174</v>
       </c>
       <c r="D116" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E116" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F116" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
     </row>
     <row r="117" spans="3:6" x14ac:dyDescent="0.25">
@@ -5499,13 +5543,13 @@
         <v>175</v>
       </c>
       <c r="D117" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E117" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F117" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
     </row>
     <row r="118" spans="3:6" x14ac:dyDescent="0.25">
@@ -5513,13 +5557,13 @@
         <v>176</v>
       </c>
       <c r="D118" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E118" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F118" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
     </row>
     <row r="119" spans="3:6" x14ac:dyDescent="0.25">
@@ -5527,13 +5571,13 @@
         <v>177</v>
       </c>
       <c r="D119" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E119" t="s">
         <v>119</v>
       </c>
       <c r="F119" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
     </row>
     <row r="120" spans="3:6" x14ac:dyDescent="0.25">
@@ -5541,13 +5585,13 @@
         <v>178</v>
       </c>
       <c r="D120" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E120" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F120" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="121" spans="3:6" x14ac:dyDescent="0.25">
@@ -5555,13 +5599,13 @@
         <v>179</v>
       </c>
       <c r="D121" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E121" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F121" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
     </row>
     <row r="122" spans="3:6" x14ac:dyDescent="0.25">
@@ -5569,13 +5613,13 @@
         <v>180</v>
       </c>
       <c r="D122" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E122" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F122" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
     </row>
     <row r="123" spans="3:6" x14ac:dyDescent="0.25">
@@ -5583,296 +5627,296 @@
         <v>181</v>
       </c>
       <c r="D123" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E123" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F123" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="124" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D124" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E124" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F124" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
     </row>
     <row r="125" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E125" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F125" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
     </row>
     <row r="126" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E126" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F126" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
     </row>
     <row r="127" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E127" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F127" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
     </row>
     <row r="128" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E128" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F128" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
     </row>
     <row r="129" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D129" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E129" t="s">
         <v>122</v>
       </c>
       <c r="F129" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
     </row>
     <row r="130" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D130" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E130" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F130" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="131" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E131" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F131" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
     </row>
     <row r="132" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E132" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F132" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="133" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E133" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F133" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="134" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D134" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E134" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F134" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
     </row>
     <row r="135" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D135" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E135" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F135" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="136" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D136" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E136" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F136" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="137" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D137" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E137" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F137" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
     </row>
     <row r="138" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D138" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E138" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F138" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="139" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D139" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E139" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F139" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="140" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E140" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F140" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
     </row>
     <row r="141" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E141" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F141" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="142" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E142" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F142" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="143" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E143" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F143" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="144" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D144" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E144" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F144" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="145" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D145" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E145" t="s">
         <v>134</v>
       </c>
       <c r="F145" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
     </row>
     <row r="146" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D146" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E146" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F146" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="147" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E147" t="s">
         <v>138</v>
       </c>
       <c r="F147" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
     </row>
     <row r="148" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E148" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F148" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="149" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D149" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E149" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F149" t="s">
         <v>174</v>
@@ -5880,419 +5924,419 @@
     </row>
     <row r="150" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D150" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E150" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F150" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
     </row>
     <row r="151" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D151" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E151" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F151" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
     </row>
     <row r="152" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D152" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E152" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F152" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
     </row>
     <row r="153" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D153" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E153" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F153" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="154" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D154" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E154" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F154" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
     </row>
     <row r="155" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D155" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E155" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F155" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
     </row>
     <row r="156" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D156" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E156" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F156" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
     </row>
     <row r="157" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D157" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E157" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F157" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
     </row>
     <row r="158" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D158" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E158" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F158" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="159" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D159" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E159" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F159" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="160" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D160" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E160" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F160" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
     </row>
     <row r="161" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D161" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E161" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="162" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D162" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E162" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="163" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D163" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E163" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="164" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D164" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E164" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="165" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D165" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E165" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="166" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D166" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E166" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="167" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D167" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E167" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="168" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D168" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E168" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="169" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D169" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E169" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="170" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D170" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E170" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="171" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D171" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E171" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="172" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D172" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E172" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="173" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D173" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E173" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="174" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D174" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E174" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="175" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D175" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E175" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="176" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D176" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E176" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="177" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D177" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E177" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="178" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D178" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E178" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="179" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D179" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E179" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="180" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D180" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E180" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="181" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D181" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E181" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="182" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D182" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E182" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="183" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D183" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E183" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="184" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D184" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E184" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="185" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D185" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E185" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="186" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D186" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E186" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="187" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D187" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E187" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="188" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D188" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E188" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="189" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D189" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E189" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="190" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D190" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E190" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="191" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D191" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E191" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="192" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D192" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E192" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="193" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D193" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E193" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="194" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D194" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E194" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="195" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D195" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E195" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="196" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D196" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E196" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="197" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D197" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E197" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="198" spans="4:5" x14ac:dyDescent="0.25">
@@ -6300,284 +6344,284 @@
         <v>140</v>
       </c>
       <c r="E198" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="199" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D199" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E199" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="200" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D200" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E200" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="201" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D201" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E201" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="202" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D202" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E202" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="203" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D203" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E203" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="204" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D204" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E204" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="205" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D205" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E205" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="206" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D206" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E206" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="207" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D207" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E207" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="208" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D208" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E208" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="209" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D209" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E209" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="210" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D210" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E210" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="211" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D211" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E211" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="212" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D212" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E212" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="213" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D213" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E213" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="214" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D214" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E214" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="215" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D215" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E215" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="216" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D216" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E216" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="217" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D217" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E217" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="218" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D218" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E218" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="219" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D219" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E219" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="220" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D220" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E220" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="221" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D221" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E221" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="222" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D222" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E222" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="223" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D223" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E223" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="224" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D224" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E224" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="225" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D225" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E225" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="226" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D226" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E226" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="227" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D227" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E227" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="228" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D228" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E228" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="229" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D229" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E229" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="230" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D230" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E230" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="231" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D231" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E231" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="232" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D232" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E232" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="233" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D233" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E233" t="s">
         <v>174</v>
@@ -6585,286 +6629,286 @@
     </row>
     <row r="234" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D234" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E234" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="235" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D235" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E235" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="236" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D236" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E236" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="237" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D237" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E237" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="238" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D238" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E238" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="239" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D239" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E239" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="240" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D240" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E240" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="241" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D241" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E241" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="242" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D242" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E242" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="243" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D243" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E243" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="244" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D244" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E244" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="245" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D245" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E245" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="246" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D246" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E246" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="247" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D247" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E247" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="248" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D248" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="E248" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="249" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D249" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E249" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="250" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D250" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E250" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="251" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D251" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E251" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="252" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D252" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E252" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="253" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D253" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E253" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="254" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D254" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E254" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="255" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D255" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E255" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="256" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D256" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E256" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="257" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D257" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E257" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="258" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D258" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E258" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
     </row>
     <row r="259" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D259" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E259" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
     </row>
     <row r="260" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D260" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E260" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
     </row>
     <row r="261" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D261" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E261" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
     </row>
     <row r="262" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D262" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="263" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D263" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="264" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D264" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="265" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D265" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="266" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D266" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="267" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D267" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="268" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D268" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="269" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D269" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="270" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D270" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="271" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D271" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="272" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D272" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="273" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D273" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added data validation rules for 2 additional fields
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet1.xlsx
+++ b/xlsx/sample-spreadsheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D32B22-EED5-44F3-ACA8-6205619D45A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903AECA8-52EC-4505-A163-8B7417B34493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="839">
   <si>
     <t>Municipality</t>
   </si>
@@ -2530,13 +2530,31 @@
   </si>
   <si>
     <t>Bicycle/Pedestrian Facility</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>EB</t>
+  </si>
+  <si>
+    <t>WB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2556,6 +2574,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2641,13 +2665,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}" name="Table5" displayName="Table5" ref="D1:G273" totalsRowShown="0">
-  <autoFilter ref="D1:G273" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}" name="Table5" displayName="Table5" ref="D1:H273" totalsRowShown="0">
+  <autoFilter ref="D1:H273" xr:uid="{7CCEC514-50DC-4567-BC60-8446CFB20D16}"/>
+  <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{09935779-A7F4-4E95-BF0B-6D7F0A5AF862}" name="Count Location Description"/>
     <tableColumn id="2" xr3:uid="{588C097D-696D-4C7A-AB98-CC5016F219D2}" name="Street #1 Name"/>
     <tableColumn id="3" xr3:uid="{CA556A4C-1BD7-4427-8132-618C09C12162}" name="Street #2 Name"/>
     <tableColumn id="4" xr3:uid="{C9E4663B-CFA0-49B0-ABFE-EA028F045F02}" name="Column1"/>
+    <tableColumn id="5" xr3:uid="{10804406-D5D0-4115-A66B-01E0B7201282}" name="Column2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2953,7 +2978,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3034,7 +3059,7 @@
         <v>818</v>
       </c>
       <c r="B8" t="s">
-        <v>458</v>
+        <v>833</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -3054,7 +3079,7 @@
         <v>817</v>
       </c>
       <c r="B10" t="s">
-        <v>464</v>
+        <v>833</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -3106,7 +3131,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CBF8E227-3C60-4987-AFCD-93955E6231E2}">
           <x14:formula1>
             <xm:f>Columns!$A$2:$A$57</xm:f>
@@ -3135,19 +3160,25 @@
           <x14:formula1>
             <xm:f>Columns!$E$2:$E$261</xm:f>
           </x14:formula1>
-          <xm:sqref>B7:B8</xm:sqref>
+          <xm:sqref>B7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1B40AB95-73FE-4909-8424-F73F83C41E06}">
           <x14:formula1>
             <xm:f>Columns!$F$2:$F$160</xm:f>
           </x14:formula1>
-          <xm:sqref>B9:B10</xm:sqref>
+          <xm:sqref>B9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{673A9766-EB25-4266-BAB5-BD22FA753598}">
           <x14:formula1>
             <xm:f>Columns!$G$2:$G$6</xm:f>
           </x14:formula1>
           <xm:sqref>B12</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1EF78375-2AFE-4EBF-9E95-4F68CFC74C8B}">
+          <x14:formula1>
+            <xm:f>Columns!$H$2:$H$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B8 B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3699,10 +3730,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F92867D1-D2E9-42B4-B903-CE81613CFB5C}">
-  <dimension ref="A1:G273"/>
+  <dimension ref="A1:H273"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3716,7 +3747,7 @@
     <col min="7" max="7" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3738,8 +3769,11 @@
       <c r="G1" t="s">
         <v>827</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3761,8 +3795,11 @@
       <c r="G2" t="s">
         <v>826</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3784,8 +3821,11 @@
       <c r="G3" t="s">
         <v>828</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3804,8 +3844,11 @@
       <c r="G4" t="s">
         <v>829</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3824,8 +3867,11 @@
       <c r="G5" t="s">
         <v>830</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -3844,8 +3890,11 @@
       <c r="G6" t="s">
         <v>831</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -3862,7 +3911,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -3879,7 +3928,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -3896,7 +3945,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -3913,7 +3962,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -3930,7 +3979,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -3947,7 +3996,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -3964,7 +4013,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -3981,7 +4030,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -3998,7 +4047,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -6912,6 +6961,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="2">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Added some values for testing
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet1.xlsx
+++ b/xlsx/sample-spreadsheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{903AECA8-52EC-4505-A163-8B7417B34493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD63B47-73D2-4BCD-9E61-8C58AE4EF4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="839">
   <si>
     <t>Municipality</t>
   </si>
@@ -2978,7 +2978,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3087,11 +3087,17 @@
       <c r="A11" s="1" t="s">
         <v>813</v>
       </c>
+      <c r="B11">
+        <v>65</v>
+      </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>814</v>
+      </c>
+      <c r="B12" t="s">
+        <v>828</v>
       </c>
       <c r="D12" s="1"/>
     </row>

</xml_diff>

<commit_message>
More values for testing
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet1.xlsx
+++ b/xlsx/sample-spreadsheet1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD63B47-73D2-4BCD-9E61-8C58AE4EF4B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF16787-5097-4140-B74D-4A56EE123580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="839">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="840">
   <si>
     <t>Municipality</t>
   </si>
@@ -2548,6 +2548,9 @@
   </si>
   <si>
     <t>WB</t>
+  </si>
+  <si>
+    <t>This is a test comment.</t>
   </si>
 </sst>
 </file>
@@ -2978,7 +2981,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A15" sqref="A15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3111,7 +3114,9 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
+      <c r="A15" s="9" t="s">
+        <v>839</v>
+      </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>

</xml_diff>

<commit_message>
Populated tab 1 with sample data
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet1.xlsx
+++ b/xlsx/sample-spreadsheet1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF16787-5097-4140-B74D-4A56EE123580}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9960EEBD-2E23-4288-9C85-767D5A0E8511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="840">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="841">
   <si>
     <t>Municipality</t>
   </si>
@@ -2551,6 +2551,9 @@
   </si>
   <si>
     <t>This is a test comment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -2980,7 +2983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D396DD5C-31B0-418A-83C6-51CCF2B5706A}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15:D16"/>
     </sheetView>
   </sheetViews>
@@ -3201,8 +3204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF117DD8-8B54-44CC-AA12-FC16BF191D23}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3243,68 +3246,242 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>200</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0.28125</v>
       </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
       <c r="C3">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>40</v>
+      </c>
+      <c r="F3">
         <v>2</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0.29166666666666669</v>
       </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>17</v>
+      </c>
       <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="F4">
         <v>3</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>0.30208333333333331</v>
       </c>
+      <c r="B5">
+        <v>33</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>400</v>
+      </c>
       <c r="E5">
+        <v>60</v>
+      </c>
+      <c r="F5">
         <v>4</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>0.3125</v>
       </c>
+      <c r="B6">
+        <v>44</v>
+      </c>
+      <c r="C6">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+      <c r="E6">
+        <v>70</v>
+      </c>
       <c r="F6">
         <v>5</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>0.32291666666666669</v>
       </c>
+      <c r="B7" t="s">
+        <v>840</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>600</v>
+      </c>
+      <c r="E7">
+        <v>80</v>
+      </c>
       <c r="G7">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>0.33333333333333331</v>
       </c>
-      <c r="H8">
+      <c r="B8">
+        <v>66</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>700</v>
+      </c>
+      <c r="E8">
+        <v>90</v>
+      </c>
+      <c r="F8">
         <v>7</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>840</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>0.34375</v>
       </c>
+      <c r="B9">
+        <v>77</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>800</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>11</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>0.35416666666666669</v>
       </c>
+      <c r="B10">
+        <v>88</v>
+      </c>
+      <c r="D10">
+        <v>900</v>
+      </c>
+      <c r="E10">
+        <v>110</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>0.36458333333333331</v>
+      </c>
+      <c r="B11">
+        <v>99</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>1000</v>
+      </c>
+      <c r="E11">
+        <v>120</v>
+      </c>
+      <c r="F11">
+        <v>9</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -3317,7 +3494,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Sample data in all 'count' tabs
</commit_message>
<xml_diff>
--- a/xlsx/sample-spreadsheet1.xlsx
+++ b/xlsx/sample-spreadsheet1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben_k\work_stuff\process-bp-count-spreadsheets\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9960EEBD-2E23-4288-9C85-767D5A0E8511}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E019BF-7862-41A2-B8D0-C884CDAAE987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="1" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="5" xr2:uid="{0C6062F5-86F8-4814-A110-428A3D225A11}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="841">
   <si>
     <t>Municipality</t>
   </si>
@@ -3204,7 +3204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF117DD8-8B54-44CC-AA12-FC16BF191D23}">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -3494,7 +3494,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="H2" sqref="H2:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3536,60 +3536,312 @@
       <c r="A2" s="6">
         <v>0.375</v>
       </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>13</v>
+      </c>
+      <c r="G2">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0.38541666666666669</v>
       </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0.39583333333333331</v>
       </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>13</v>
+      </c>
+      <c r="G4">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>0.40625</v>
       </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>0.41666666666666669</v>
       </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>13</v>
+      </c>
+      <c r="G6">
+        <v>14</v>
+      </c>
+      <c r="H6">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>0.42708333333333331</v>
       </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>13</v>
+      </c>
+      <c r="G7">
+        <v>14</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>0.4375</v>
       </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>13</v>
+      </c>
+      <c r="G8">
+        <v>14</v>
+      </c>
+      <c r="H8">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>0.44791666666666669</v>
       </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>11</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>0.45833333333333331</v>
       </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>11</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>0.46875</v>
       </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>14</v>
+      </c>
+      <c r="H11">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>0.47916666666666669</v>
       </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>13</v>
+      </c>
+      <c r="G12">
+        <v>14</v>
+      </c>
+      <c r="H12">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>0.48958333333333331</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -3602,7 +3854,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B13" sqref="B13:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3643,60 +3895,312 @@
       <c r="A2" s="6">
         <v>0.5</v>
       </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0.51041666666666663</v>
       </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>13</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0.52083333333333337</v>
       </c>
+      <c r="B4">
+        <v>14</v>
+      </c>
+      <c r="C4">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>14</v>
+      </c>
+      <c r="E4">
+        <v>14</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>14</v>
+      </c>
+      <c r="H4">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>0.53125</v>
       </c>
+      <c r="B5">
+        <v>15</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>15</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>15</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>0.54166666666666663</v>
       </c>
+      <c r="B6">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <v>16</v>
+      </c>
+      <c r="H6">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>0.55208333333333337</v>
       </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7">
+        <v>17</v>
+      </c>
+      <c r="G7">
+        <v>17</v>
+      </c>
+      <c r="H7">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>0.5625</v>
       </c>
+      <c r="B8">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>18</v>
+      </c>
+      <c r="D8">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8">
+        <v>18</v>
+      </c>
+      <c r="G8">
+        <v>18</v>
+      </c>
+      <c r="H8">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>0.57291666666666663</v>
       </c>
+      <c r="B9">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>19</v>
+      </c>
+      <c r="D9">
+        <v>19</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>19</v>
+      </c>
+      <c r="G9">
+        <v>19</v>
+      </c>
+      <c r="H9">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>0.58333333333333337</v>
       </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+      <c r="G10">
+        <v>20</v>
+      </c>
+      <c r="H10">
+        <v>20</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>0.59375</v>
       </c>
+      <c r="B11">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>21</v>
+      </c>
+      <c r="F11">
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <v>21</v>
+      </c>
+      <c r="H11">
+        <v>21</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>0.60416666666666663</v>
       </c>
+      <c r="B12">
+        <v>22</v>
+      </c>
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>22</v>
+      </c>
+      <c r="F12">
+        <v>22</v>
+      </c>
+      <c r="G12">
+        <v>22</v>
+      </c>
+      <c r="H12">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>0.61458333333333337</v>
+      </c>
+      <c r="B13">
+        <v>23</v>
+      </c>
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>23</v>
+      </c>
+      <c r="E13">
+        <v>23</v>
+      </c>
+      <c r="F13">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>23</v>
+      </c>
+      <c r="H13">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3709,7 +4213,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3749,60 +4253,312 @@
       <c r="A2" s="6">
         <v>0.625</v>
       </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0.63541666666666663</v>
       </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>100</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0.64583333333333337</v>
       </c>
+      <c r="B4">
+        <v>100</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>0.65625</v>
       </c>
+      <c r="B5">
+        <v>100</v>
+      </c>
+      <c r="C5">
+        <v>100</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>0.66666666666666663</v>
       </c>
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="D6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>0.67708333333333337</v>
       </c>
+      <c r="B7">
+        <v>100</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>0.6875</v>
       </c>
+      <c r="B8">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>100</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>0.69791666666666663</v>
       </c>
+      <c r="B9">
+        <v>100</v>
+      </c>
+      <c r="C9">
+        <v>100</v>
+      </c>
+      <c r="D9">
+        <v>100</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>100</v>
+      </c>
+      <c r="G9">
+        <v>100</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>0.70833333333333337</v>
       </c>
+      <c r="B10">
+        <v>100</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>100</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>100</v>
+      </c>
+      <c r="G10">
+        <v>100</v>
+      </c>
+      <c r="H10">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>0.71875</v>
       </c>
+      <c r="B11">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>100</v>
+      </c>
+      <c r="D11">
+        <v>100</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+      <c r="G11">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>100</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>0.72916666666666663</v>
       </c>
+      <c r="B12">
+        <v>100</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12">
+        <v>100</v>
+      </c>
+      <c r="H12">
+        <v>100</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>0.73958333333333337</v>
+      </c>
+      <c r="B13">
+        <v>100</v>
+      </c>
+      <c r="C13">
+        <v>100</v>
+      </c>
+      <c r="D13">
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>100</v>
+      </c>
+      <c r="H13">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3814,8 +4570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06DF4321-62D8-46CC-809D-E3E73DB3DDEB}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3855,60 +4611,300 @@
       <c r="A2" s="6">
         <v>0.75</v>
       </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>0.76041666666666663</v>
       </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <v>8</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>0.77083333333333337</v>
       </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>6</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>0.78125</v>
       </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>0.79166666666666663</v>
       </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>0.80208333333333337</v>
       </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>11</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>0.8125</v>
       </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>0.82291666666666663</v>
       </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>14</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>0.83333333333333337</v>
       </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>13</v>
+      </c>
+      <c r="G10">
+        <v>14</v>
+      </c>
+      <c r="H10">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>0.84375</v>
       </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>840</v>
+      </c>
+      <c r="F11">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>16</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>0.85416666666666663</v>
       </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <v>13</v>
+      </c>
+      <c r="E12">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>16</v>
+      </c>
+      <c r="H12">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>0.86458333333333337</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>16</v>
+      </c>
+      <c r="H13">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>